<commit_message>
sankarin liike animaatio toimii nyt oikein. JEEEEEEEEEEEEEEEEEEEEEE
</commit_message>
<xml_diff>
--- a/documents/Sprintin tehtävälista.xlsx
+++ b/documents/Sprintin tehtävälista.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670"/>
   </bookViews>
   <sheets>
     <sheet name="Sprintin tehtävälista" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Get Status</t>
   </si>
@@ -540,7 +540,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -713,11 +712,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145339520"/>
-        <c:axId val="145341440"/>
+        <c:axId val="90952448"/>
+        <c:axId val="90954368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145339520"/>
+        <c:axId val="90952448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,14 +738,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145341440"/>
+        <c:crossAx val="90954368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145341440"/>
+        <c:axId val="90954368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,21 +775,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145339520"/>
+        <c:crossAx val="90952448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1140,11 +1136,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1352,6 +1348,12 @@
       <c r="B13" s="31" t="s">
         <v>46</v>
       </c>
+      <c r="C13" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
@@ -1490,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1649,7 +1651,7 @@
       </c>
       <c r="C4" s="32">
         <f ca="1">TODAY()</f>
-        <v>41346</v>
+        <v>41360</v>
       </c>
       <c r="D4" s="8"/>
       <c r="I4" s="3"/>

</xml_diff>